<commit_message>
Corrections to flexibility points provided by pumped hydro (repurposed geothermal)
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BPaFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85F64E1-EA80-4F7B-A529-47493BB04454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
     <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Source:</t>
   </si>
@@ -151,9 +156,6 @@
     <t>in India they are are used for peaking as well as a low level of baseload.</t>
   </si>
   <si>
-    <t>For India, Flag zero for hydro because we track pumped hydro separately.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Petroleum/diesel plants are flagged as 1 as they are used for balancing </t>
   </si>
   <si>
@@ -173,12 +175,21 @@
   </si>
   <si>
     <t>In the India EPS, the geothermal plant type is repurposed as pumped hydro capacity.</t>
+  </si>
+  <si>
+    <t>For India, Flag zero for hydro because we track pumped hydro separately</t>
+  </si>
+  <si>
+    <t>the flexibility points as peaker plants, we use a value of 0.5 for geothermal here.</t>
+  </si>
+  <si>
+    <t>as the geothermal plant type. Because pumped hydro plants provide half (see elec/FPC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -327,6 +338,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -362,6 +390,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,26 +582,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,151 +609,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -728,17 +783,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.265625" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -746,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -754,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -762,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -770,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -778,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -786,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -794,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -802,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -810,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -818,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -826,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -835,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -844,25 +899,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>45</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -874,27 +929,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.265625" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -902,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -910,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -918,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -926,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -934,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -942,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -950,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -958,15 +1013,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -974,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -982,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -991,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1000,25 +1055,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>45</v>
       </c>
       <c r="B17">
         <v>0</v>

</xml_diff>

<commit_message>
Corresponding edits from low GDP (develop) branch
</commit_message>
<xml_diff>
--- a/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
+++ b/InputData/elec/BPaFF/Boolean Peaking and Flexibility Flags.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BPaFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\elec\BPaFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85F64E1-EA80-4F7B-A529-47493BB04454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BPaFF-BITPTaP" sheetId="2" r:id="rId2"/>
     <sheet name="BPaFF-BDTPTPF" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Source:</t>
   </si>
@@ -151,9 +156,6 @@
     <t>in India they are are used for peaking as well as a low level of baseload.</t>
   </si>
   <si>
-    <t>For India, Flag zero for hydro because we track pumped hydro separately.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Petroleum/diesel plants are flagged as 1 as they are used for balancing </t>
   </si>
   <si>
@@ -173,12 +175,21 @@
   </si>
   <si>
     <t>In the India EPS, the geothermal plant type is repurposed as pumped hydro capacity.</t>
+  </si>
+  <si>
+    <t>For India, Flag zero for hydro because we track pumped hydro separately</t>
+  </si>
+  <si>
+    <t>the flexibility points as peaker plants, we use a value of 0.5 for geothermal here.</t>
+  </si>
+  <si>
+    <t>as the geothermal plant type. Because pumped hydro plants provide half (see elec/FPC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -327,6 +338,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -362,6 +390,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,26 +582,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,151 +609,161 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -728,17 +783,17 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.265625" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -746,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -754,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -762,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -770,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -778,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -786,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -794,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -802,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -810,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -818,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -826,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -835,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -844,25 +899,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>45</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -874,27 +929,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.265625" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -902,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -910,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -918,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -926,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -934,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -942,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -950,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -958,15 +1013,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -974,7 +1029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -982,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -991,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1000,25 +1055,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>44</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>45</v>
       </c>
       <c r="B17">
         <v>0</v>

</xml_diff>